<commit_message>
added more ge11 registers to pcie_address_table
</commit_message>
<xml_diff>
--- a/emtf_v7/doc/pcie_address_table/emtf_pcie_address_table.xlsx
+++ b/emtf_v7/doc/pcie_address_table/emtf_pcie_address_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\madorsky\github\vivado\emtf\emtf_v7\doc\pcie_address_table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700AF75C-FBF4-4CC8-8FBF-DE4C8301B430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E057713-95FA-4173-BC9A-5F3BDA5D0B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11577" uniqueCount="901">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11787" uniqueCount="925">
   <si>
     <t>// path</t>
   </si>
@@ -2740,6 +2740,78 @@
   </si>
   <si>
     <t>25</t>
+  </si>
+  <si>
+    <t>GE1/1 manual delay</t>
+  </si>
+  <si>
+    <t>ge11_af manual_delay</t>
+  </si>
+  <si>
+    <t>GE1/1 auto delay</t>
+  </si>
+  <si>
+    <t>ge11_af auto_delay</t>
+  </si>
+  <si>
+    <t>GE1/1 auto delay out of range</t>
+  </si>
+  <si>
+    <t>0000000800000000</t>
+  </si>
+  <si>
+    <t>0000004000000000</t>
+  </si>
+  <si>
+    <t>0000008000000000</t>
+  </si>
+  <si>
+    <t>0000010000000000</t>
+  </si>
+  <si>
+    <t>0000020000000000</t>
+  </si>
+  <si>
+    <t>GE1/1 BC0 period error</t>
+  </si>
+  <si>
+    <t>0000040000000000</t>
+  </si>
+  <si>
+    <t>0000080000000000</t>
+  </si>
+  <si>
+    <t>0000100000000000</t>
+  </si>
+  <si>
+    <t>0000200000000000</t>
+  </si>
+  <si>
+    <t>0000400000000000</t>
+  </si>
+  <si>
+    <t>0000800000000000</t>
+  </si>
+  <si>
+    <t>0001000000000000</t>
+  </si>
+  <si>
+    <t>ge11_af_auto_out_of_range</t>
+  </si>
+  <si>
+    <t>ge11_bc0_period_err</t>
+  </si>
+  <si>
+    <t>GE1/1 BC0 delay</t>
+  </si>
+  <si>
+    <t>GE1/1 enable manual alignment delay</t>
+  </si>
+  <si>
+    <t>ge11_bc0_delay</t>
+  </si>
+  <si>
+    <t>ge11_en_manual_af_delay</t>
   </si>
 </sst>
 </file>
@@ -2878,7 +2950,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2930,6 +3002,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3312,11 +3386,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:IW1514"/>
+  <dimension ref="A1:IW1547"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A552" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J579" sqref="J579"/>
+      <pane ySplit="1" topLeftCell="A1498" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N1537" sqref="N1537"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -74305,28 +74379,28 @@
       <c r="M1504" s="10"/>
       <c r="N1504" s="10"/>
     </row>
-    <row r="1505" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1505" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1505" s="8" t="s">
         <v>118</v>
       </c>
       <c r="B1505" s="9">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C1505" s="9">
         <v>0</v>
       </c>
       <c r="D1505" s="9">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="E1505" s="10" t="str">
         <f t="shared" ref="E1505" si="225">DEC2HEX(HEX2DEC(A1505)+B1505*4096+HEX2DEC(D1505)*8,8)</f>
-        <v>000B7000</v>
+        <v>000B6390</v>
       </c>
       <c r="F1505" s="8" t="s">
-        <v>885</v>
+        <v>90</v>
       </c>
       <c r="G1505" s="8" t="s">
-        <v>22</v>
+        <v>324</v>
       </c>
       <c r="H1505" s="8" t="s">
         <v>23</v>
@@ -74335,37 +74409,43 @@
         <v>23</v>
       </c>
       <c r="J1505" s="16" t="s">
-        <v>883</v>
-      </c>
-      <c r="K1505" s="26"/>
+        <v>901</v>
+      </c>
+      <c r="K1505" s="26">
+        <v>0</v>
+      </c>
       <c r="L1505" s="11"/>
       <c r="M1505" s="10"/>
-      <c r="N1505" s="10" t="s">
-        <v>884</v>
-      </c>
-    </row>
-    <row r="1506" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N1505" s="10" t="str">
+        <f t="shared" ref="N1505" si="226">CONCATENATE(O1505,"_",K1505)</f>
+        <v>ge11_af manual_delay_0</v>
+      </c>
+      <c r="O1505" s="3" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="1506" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1506" s="8" t="s">
         <v>118</v>
       </c>
       <c r="B1506" s="9">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C1506" s="9">
         <v>0</v>
       </c>
       <c r="D1506" s="9">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="E1506" s="10" t="str">
-        <f t="shared" ref="E1506" si="226">DEC2HEX(HEX2DEC(A1506)+B1506*4096+HEX2DEC(D1506)*8,8)</f>
-        <v>000B8000</v>
+        <f t="shared" ref="E1506:E1511" si="227">DEC2HEX(HEX2DEC(A1506)+B1506*4096+HEX2DEC(D1506)*8,8)</f>
+        <v>000B6390</v>
       </c>
       <c r="F1506" s="8" t="s">
-        <v>885</v>
+        <v>90</v>
       </c>
       <c r="G1506" s="8" t="s">
-        <v>22</v>
+        <v>327</v>
       </c>
       <c r="H1506" s="8" t="s">
         <v>23</v>
@@ -74374,216 +74454,1596 @@
         <v>23</v>
       </c>
       <c r="J1506" s="16" t="s">
-        <v>886</v>
-      </c>
-      <c r="K1506" s="26"/>
+        <v>901</v>
+      </c>
+      <c r="K1506" s="26">
+        <v>1</v>
+      </c>
       <c r="L1506" s="11"/>
       <c r="M1506" s="10"/>
-      <c r="N1506" s="10" t="s">
-        <v>887</v>
-      </c>
-    </row>
-    <row r="1507" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1507" s="8"/>
-      <c r="B1507" s="9"/>
-      <c r="C1507" s="9"/>
-      <c r="D1507" s="9"/>
-      <c r="E1507" s="10"/>
-      <c r="F1507" s="8"/>
-      <c r="G1507" s="10"/>
-      <c r="H1507" s="8"/>
-      <c r="I1507" s="8"/>
-      <c r="J1507" s="8"/>
-      <c r="K1507" s="10"/>
+      <c r="N1506" s="10" t="str">
+        <f t="shared" ref="N1506:N1511" si="228">CONCATENATE(O1506,"_",K1506)</f>
+        <v>ge11_af manual_delay_1</v>
+      </c>
+      <c r="O1506" s="3" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="1507" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1507" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1507" s="9">
+        <v>54</v>
+      </c>
+      <c r="C1507" s="9">
+        <v>0</v>
+      </c>
+      <c r="D1507" s="9">
+        <v>72</v>
+      </c>
+      <c r="E1507" s="10" t="str">
+        <f t="shared" si="227"/>
+        <v>000B6390</v>
+      </c>
+      <c r="F1507" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1507" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="H1507" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1507" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1507" s="16" t="s">
+        <v>901</v>
+      </c>
+      <c r="K1507" s="26">
+        <v>2</v>
+      </c>
       <c r="L1507" s="11"/>
       <c r="M1507" s="10"/>
-      <c r="N1507" s="10"/>
-    </row>
-    <row r="1508" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N1507" s="10" t="str">
+        <f t="shared" si="228"/>
+        <v>ge11_af manual_delay_2</v>
+      </c>
+      <c r="O1507" s="3" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="1508" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1508" s="8" t="s">
-        <v>859</v>
-      </c>
-      <c r="B1508" s="9"/>
-      <c r="C1508" s="9"/>
-      <c r="D1508" s="8"/>
-      <c r="E1508" s="10" t="s">
-        <v>860</v>
+        <v>118</v>
+      </c>
+      <c r="B1508" s="9">
+        <v>54</v>
+      </c>
+      <c r="C1508" s="9">
+        <v>0</v>
+      </c>
+      <c r="D1508" s="9">
+        <v>72</v>
+      </c>
+      <c r="E1508" s="10" t="str">
+        <f t="shared" si="227"/>
+        <v>000B6390</v>
       </c>
       <c r="F1508" s="8" t="s">
-        <v>861</v>
+        <v>90</v>
       </c>
       <c r="G1508" s="8" t="s">
-        <v>862</v>
+        <v>333</v>
       </c>
       <c r="H1508" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I1508" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1508" s="8" t="s">
-        <v>863</v>
-      </c>
-      <c r="K1508" s="10"/>
-      <c r="L1508" s="8"/>
+      <c r="I1508" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1508" s="16" t="s">
+        <v>901</v>
+      </c>
+      <c r="K1508" s="26">
+        <v>3</v>
+      </c>
+      <c r="L1508" s="11"/>
       <c r="M1508" s="10"/>
-      <c r="N1508" s="10" t="s">
-        <v>864</v>
-      </c>
-    </row>
-    <row r="1509" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N1508" s="10" t="str">
+        <f t="shared" si="228"/>
+        <v>ge11_af manual_delay_3</v>
+      </c>
+      <c r="O1508" s="3" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="1509" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1509" s="8" t="s">
-        <v>859</v>
-      </c>
-      <c r="B1509" s="9"/>
-      <c r="C1509" s="9"/>
-      <c r="D1509" s="8"/>
-      <c r="E1509" s="8" t="s">
-        <v>865</v>
+        <v>118</v>
+      </c>
+      <c r="B1509" s="9">
+        <v>54</v>
+      </c>
+      <c r="C1509" s="9">
+        <v>0</v>
+      </c>
+      <c r="D1509" s="9">
+        <v>72</v>
+      </c>
+      <c r="E1509" s="10" t="str">
+        <f t="shared" si="227"/>
+        <v>000B6390</v>
       </c>
       <c r="F1509" s="8" t="s">
-        <v>861</v>
+        <v>90</v>
       </c>
       <c r="G1509" s="8" t="s">
-        <v>862</v>
+        <v>825</v>
       </c>
       <c r="H1509" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I1509" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1509" s="8" t="s">
-        <v>866</v>
-      </c>
-      <c r="K1509" s="10"/>
-      <c r="L1509" s="8"/>
+      <c r="I1509" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1509" s="16" t="s">
+        <v>901</v>
+      </c>
+      <c r="K1509" s="26">
+        <v>4</v>
+      </c>
+      <c r="L1509" s="11"/>
       <c r="M1509" s="10"/>
-      <c r="N1509" s="10" t="s">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="1510" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1510" s="8"/>
-      <c r="B1510" s="9"/>
-      <c r="C1510" s="9"/>
-      <c r="D1510" s="8"/>
-      <c r="E1510" s="10"/>
-      <c r="F1510" s="8"/>
-      <c r="G1510" s="8"/>
-      <c r="H1510" s="8"/>
-      <c r="I1510" s="8"/>
-      <c r="J1510" s="8"/>
-      <c r="K1510" s="10"/>
-      <c r="L1510" s="8"/>
+      <c r="N1509" s="10" t="str">
+        <f t="shared" si="228"/>
+        <v>ge11_af manual_delay_4</v>
+      </c>
+      <c r="O1509" s="3" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="1510" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1510" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1510" s="9">
+        <v>54</v>
+      </c>
+      <c r="C1510" s="9">
+        <v>0</v>
+      </c>
+      <c r="D1510" s="9">
+        <v>72</v>
+      </c>
+      <c r="E1510" s="10" t="str">
+        <f t="shared" si="227"/>
+        <v>000B6390</v>
+      </c>
+      <c r="F1510" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1510" s="8" t="s">
+        <v>826</v>
+      </c>
+      <c r="H1510" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1510" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1510" s="16" t="s">
+        <v>901</v>
+      </c>
+      <c r="K1510" s="26">
+        <v>5</v>
+      </c>
+      <c r="L1510" s="11"/>
       <c r="M1510" s="10"/>
-      <c r="N1510" s="10"/>
-    </row>
-    <row r="1511" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N1510" s="10" t="str">
+        <f t="shared" si="228"/>
+        <v>ge11_af manual_delay_5</v>
+      </c>
+      <c r="O1510" s="3" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="1511" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1511" s="8" t="s">
-        <v>868</v>
-      </c>
-      <c r="B1511" s="9"/>
-      <c r="C1511" s="9"/>
-      <c r="D1511" s="8"/>
-      <c r="E1511" s="8" t="s">
-        <v>869</v>
+        <v>118</v>
+      </c>
+      <c r="B1511" s="9">
+        <v>54</v>
+      </c>
+      <c r="C1511" s="9">
+        <v>0</v>
+      </c>
+      <c r="D1511" s="9">
+        <v>72</v>
+      </c>
+      <c r="E1511" s="10" t="str">
+        <f t="shared" si="227"/>
+        <v>000B6390</v>
       </c>
       <c r="F1511" s="8" t="s">
-        <v>870</v>
+        <v>90</v>
       </c>
       <c r="G1511" s="8" t="s">
-        <v>22</v>
+        <v>827</v>
       </c>
       <c r="H1511" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I1511" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1511" s="8" t="s">
-        <v>871</v>
-      </c>
-      <c r="K1511" s="10"/>
-      <c r="L1511" s="8"/>
+      <c r="I1511" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1511" s="16" t="s">
+        <v>901</v>
+      </c>
+      <c r="K1511" s="26">
+        <v>6</v>
+      </c>
+      <c r="L1511" s="11"/>
       <c r="M1511" s="10"/>
-      <c r="N1511" s="10" t="s">
-        <v>872</v>
-      </c>
-    </row>
-    <row r="1512" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N1511" s="10" t="str">
+        <f t="shared" si="228"/>
+        <v>ge11_af manual_delay_6</v>
+      </c>
+      <c r="O1511" s="3" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="1512" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1512" s="8"/>
       <c r="B1512" s="9"/>
       <c r="C1512" s="9"/>
-      <c r="D1512" s="8"/>
+      <c r="D1512" s="9"/>
       <c r="E1512" s="10"/>
       <c r="F1512" s="8"/>
       <c r="G1512" s="8"/>
       <c r="H1512" s="8"/>
-      <c r="I1512" s="8"/>
-      <c r="J1512" s="8"/>
-      <c r="K1512" s="10"/>
-      <c r="L1512" s="8"/>
+      <c r="I1512" s="18"/>
+      <c r="J1512" s="29"/>
+      <c r="K1512" s="30"/>
+      <c r="L1512" s="11"/>
       <c r="M1512" s="10"/>
       <c r="N1512" s="10"/>
     </row>
-    <row r="1513" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1513" s="23"/>
-      <c r="B1513" s="27"/>
-      <c r="C1513" s="27"/>
-      <c r="D1513" s="23"/>
-      <c r="E1513" s="23" t="s">
+    <row r="1513" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1513" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1513" s="9">
+        <v>54</v>
+      </c>
+      <c r="C1513" s="9">
+        <v>0</v>
+      </c>
+      <c r="D1513" s="9">
+        <v>73</v>
+      </c>
+      <c r="E1513" s="10" t="str">
+        <f t="shared" ref="E1513:E1519" si="229">DEC2HEX(HEX2DEC(A1513)+B1513*4096+HEX2DEC(D1513)*8,8)</f>
+        <v>000B6398</v>
+      </c>
+      <c r="F1513" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1513" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="H1513" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1513" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1513" s="16" t="s">
+        <v>903</v>
+      </c>
+      <c r="K1513" s="26">
+        <v>0</v>
+      </c>
+      <c r="L1513" s="11"/>
+      <c r="M1513" s="10"/>
+      <c r="N1513" s="10" t="str">
+        <f t="shared" ref="N1513:N1519" si="230">CONCATENATE(O1513,"_",K1513)</f>
+        <v>ge11_af auto_delay_0</v>
+      </c>
+      <c r="O1513" s="3" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="1514" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1514" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1514" s="9">
+        <v>54</v>
+      </c>
+      <c r="C1514" s="9">
+        <v>0</v>
+      </c>
+      <c r="D1514" s="9">
+        <v>73</v>
+      </c>
+      <c r="E1514" s="10" t="str">
+        <f t="shared" si="229"/>
+        <v>000B6398</v>
+      </c>
+      <c r="F1514" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1514" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="H1514" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1514" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1514" s="16" t="s">
+        <v>903</v>
+      </c>
+      <c r="K1514" s="26">
+        <v>1</v>
+      </c>
+      <c r="L1514" s="11"/>
+      <c r="M1514" s="10"/>
+      <c r="N1514" s="10" t="str">
+        <f t="shared" si="230"/>
+        <v>ge11_af auto_delay_1</v>
+      </c>
+      <c r="O1514" s="3" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="1515" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1515" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1515" s="9">
+        <v>54</v>
+      </c>
+      <c r="C1515" s="9">
+        <v>0</v>
+      </c>
+      <c r="D1515" s="9">
+        <v>73</v>
+      </c>
+      <c r="E1515" s="10" t="str">
+        <f t="shared" si="229"/>
+        <v>000B6398</v>
+      </c>
+      <c r="F1515" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1515" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="H1515" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1515" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1515" s="16" t="s">
+        <v>903</v>
+      </c>
+      <c r="K1515" s="26">
+        <v>2</v>
+      </c>
+      <c r="L1515" s="11"/>
+      <c r="M1515" s="10"/>
+      <c r="N1515" s="10" t="str">
+        <f t="shared" si="230"/>
+        <v>ge11_af auto_delay_2</v>
+      </c>
+      <c r="O1515" s="3" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="1516" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1516" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1516" s="9">
+        <v>54</v>
+      </c>
+      <c r="C1516" s="9">
+        <v>0</v>
+      </c>
+      <c r="D1516" s="9">
+        <v>73</v>
+      </c>
+      <c r="E1516" s="10" t="str">
+        <f t="shared" si="229"/>
+        <v>000B6398</v>
+      </c>
+      <c r="F1516" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1516" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="H1516" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1516" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1516" s="16" t="s">
+        <v>903</v>
+      </c>
+      <c r="K1516" s="26">
+        <v>3</v>
+      </c>
+      <c r="L1516" s="11"/>
+      <c r="M1516" s="10"/>
+      <c r="N1516" s="10" t="str">
+        <f t="shared" si="230"/>
+        <v>ge11_af auto_delay_3</v>
+      </c>
+      <c r="O1516" s="3" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="1517" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1517" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1517" s="9">
+        <v>54</v>
+      </c>
+      <c r="C1517" s="9">
+        <v>0</v>
+      </c>
+      <c r="D1517" s="9">
+        <v>73</v>
+      </c>
+      <c r="E1517" s="10" t="str">
+        <f t="shared" si="229"/>
+        <v>000B6398</v>
+      </c>
+      <c r="F1517" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1517" s="8" t="s">
+        <v>825</v>
+      </c>
+      <c r="H1517" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1517" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1517" s="16" t="s">
+        <v>903</v>
+      </c>
+      <c r="K1517" s="26">
+        <v>4</v>
+      </c>
+      <c r="L1517" s="11"/>
+      <c r="M1517" s="10"/>
+      <c r="N1517" s="10" t="str">
+        <f t="shared" si="230"/>
+        <v>ge11_af auto_delay_4</v>
+      </c>
+      <c r="O1517" s="3" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="1518" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1518" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1518" s="9">
+        <v>54</v>
+      </c>
+      <c r="C1518" s="9">
+        <v>0</v>
+      </c>
+      <c r="D1518" s="9">
+        <v>73</v>
+      </c>
+      <c r="E1518" s="10" t="str">
+        <f t="shared" si="229"/>
+        <v>000B6398</v>
+      </c>
+      <c r="F1518" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1518" s="8" t="s">
+        <v>826</v>
+      </c>
+      <c r="H1518" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1518" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1518" s="16" t="s">
+        <v>903</v>
+      </c>
+      <c r="K1518" s="26">
+        <v>5</v>
+      </c>
+      <c r="L1518" s="11"/>
+      <c r="M1518" s="10"/>
+      <c r="N1518" s="10" t="str">
+        <f t="shared" si="230"/>
+        <v>ge11_af auto_delay_5</v>
+      </c>
+      <c r="O1518" s="3" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="1519" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1519" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1519" s="9">
+        <v>54</v>
+      </c>
+      <c r="C1519" s="9">
+        <v>0</v>
+      </c>
+      <c r="D1519" s="9">
+        <v>73</v>
+      </c>
+      <c r="E1519" s="10" t="str">
+        <f t="shared" si="229"/>
+        <v>000B6398</v>
+      </c>
+      <c r="F1519" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1519" s="8" t="s">
+        <v>827</v>
+      </c>
+      <c r="H1519" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1519" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1519" s="16" t="s">
+        <v>903</v>
+      </c>
+      <c r="K1519" s="26">
+        <v>6</v>
+      </c>
+      <c r="L1519" s="11"/>
+      <c r="M1519" s="10"/>
+      <c r="N1519" s="10" t="str">
+        <f t="shared" si="230"/>
+        <v>ge11_af auto_delay_6</v>
+      </c>
+      <c r="O1519" s="3" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="1520" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1520" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1520" s="9">
+        <v>54</v>
+      </c>
+      <c r="C1520" s="9">
+        <v>0</v>
+      </c>
+      <c r="D1520" s="9">
+        <v>73</v>
+      </c>
+      <c r="E1520" s="10" t="str">
+        <f t="shared" ref="E1520:E1521" si="231">DEC2HEX(HEX2DEC(A1520)+B1520*4096+HEX2DEC(D1520)*8,8)</f>
+        <v>000B6398</v>
+      </c>
+      <c r="F1520" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1520" s="8" t="s">
+        <v>906</v>
+      </c>
+      <c r="H1520" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1520" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1520" s="16" t="s">
+        <v>905</v>
+      </c>
+      <c r="K1520" s="26">
+        <v>0</v>
+      </c>
+      <c r="L1520" s="11"/>
+      <c r="M1520" s="10"/>
+      <c r="N1520" s="10" t="str">
+        <f t="shared" ref="N1520:N1521" si="232">CONCATENATE(O1520,"_",K1520)</f>
+        <v>ge11_af_auto_out_of_range_0</v>
+      </c>
+      <c r="O1520" s="3" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="1521" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1521" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1521" s="9">
+        <v>54</v>
+      </c>
+      <c r="C1521" s="9">
+        <v>0</v>
+      </c>
+      <c r="D1521" s="9">
+        <v>73</v>
+      </c>
+      <c r="E1521" s="10" t="str">
+        <f t="shared" si="231"/>
+        <v>000B6398</v>
+      </c>
+      <c r="F1521" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1521" s="8" t="s">
+        <v>635</v>
+      </c>
+      <c r="H1521" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1521" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1521" s="16" t="s">
+        <v>905</v>
+      </c>
+      <c r="K1521" s="26">
+        <v>1</v>
+      </c>
+      <c r="L1521" s="11"/>
+      <c r="M1521" s="10"/>
+      <c r="N1521" s="10" t="str">
+        <f t="shared" si="232"/>
+        <v>ge11_af_auto_out_of_range_1</v>
+      </c>
+      <c r="O1521" s="3" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="1522" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1522" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1522" s="9">
+        <v>54</v>
+      </c>
+      <c r="C1522" s="9">
+        <v>0</v>
+      </c>
+      <c r="D1522" s="9">
+        <v>73</v>
+      </c>
+      <c r="E1522" s="10" t="str">
+        <f t="shared" ref="E1522:E1528" si="233">DEC2HEX(HEX2DEC(A1522)+B1522*4096+HEX2DEC(D1522)*8,8)</f>
+        <v>000B6398</v>
+      </c>
+      <c r="F1522" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1522" s="8" t="s">
+        <v>638</v>
+      </c>
+      <c r="H1522" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1522" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1522" s="16" t="s">
+        <v>905</v>
+      </c>
+      <c r="K1522" s="26">
+        <v>2</v>
+      </c>
+      <c r="L1522" s="11"/>
+      <c r="M1522" s="10"/>
+      <c r="N1522" s="10" t="str">
+        <f t="shared" ref="N1522:N1528" si="234">CONCATENATE(O1522,"_",K1522)</f>
+        <v>ge11_af_auto_out_of_range_2</v>
+      </c>
+      <c r="O1522" s="3" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="1523" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1523" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1523" s="9">
+        <v>54</v>
+      </c>
+      <c r="C1523" s="9">
+        <v>0</v>
+      </c>
+      <c r="D1523" s="9">
+        <v>73</v>
+      </c>
+      <c r="E1523" s="10" t="str">
+        <f t="shared" si="233"/>
+        <v>000B6398</v>
+      </c>
+      <c r="F1523" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1523" s="8" t="s">
+        <v>907</v>
+      </c>
+      <c r="H1523" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1523" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1523" s="16" t="s">
+        <v>905</v>
+      </c>
+      <c r="K1523" s="26">
+        <v>3</v>
+      </c>
+      <c r="L1523" s="11"/>
+      <c r="M1523" s="10"/>
+      <c r="N1523" s="10" t="str">
+        <f t="shared" si="234"/>
+        <v>ge11_af_auto_out_of_range_3</v>
+      </c>
+      <c r="O1523" s="3" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="1524" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1524" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1524" s="9">
+        <v>54</v>
+      </c>
+      <c r="C1524" s="9">
+        <v>0</v>
+      </c>
+      <c r="D1524" s="9">
+        <v>73</v>
+      </c>
+      <c r="E1524" s="10" t="str">
+        <f t="shared" si="233"/>
+        <v>000B6398</v>
+      </c>
+      <c r="F1524" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1524" s="8" t="s">
+        <v>908</v>
+      </c>
+      <c r="H1524" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1524" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1524" s="16" t="s">
+        <v>905</v>
+      </c>
+      <c r="K1524" s="26">
+        <v>4</v>
+      </c>
+      <c r="L1524" s="11"/>
+      <c r="M1524" s="10"/>
+      <c r="N1524" s="10" t="str">
+        <f t="shared" si="234"/>
+        <v>ge11_af_auto_out_of_range_4</v>
+      </c>
+      <c r="O1524" s="3" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="1525" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1525" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1525" s="9">
+        <v>54</v>
+      </c>
+      <c r="C1525" s="9">
+        <v>0</v>
+      </c>
+      <c r="D1525" s="9">
+        <v>73</v>
+      </c>
+      <c r="E1525" s="10" t="str">
+        <f t="shared" si="233"/>
+        <v>000B6398</v>
+      </c>
+      <c r="F1525" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1525" s="8" t="s">
+        <v>909</v>
+      </c>
+      <c r="H1525" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1525" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1525" s="16" t="s">
+        <v>905</v>
+      </c>
+      <c r="K1525" s="26">
+        <v>5</v>
+      </c>
+      <c r="L1525" s="11"/>
+      <c r="M1525" s="10"/>
+      <c r="N1525" s="10" t="str">
+        <f t="shared" si="234"/>
+        <v>ge11_af_auto_out_of_range_5</v>
+      </c>
+      <c r="O1525" s="3" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="1526" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1526" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1526" s="9">
+        <v>54</v>
+      </c>
+      <c r="C1526" s="9">
+        <v>0</v>
+      </c>
+      <c r="D1526" s="9">
+        <v>73</v>
+      </c>
+      <c r="E1526" s="10" t="str">
+        <f t="shared" si="233"/>
+        <v>000B6398</v>
+      </c>
+      <c r="F1526" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1526" s="8" t="s">
+        <v>910</v>
+      </c>
+      <c r="H1526" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1526" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1526" s="16" t="s">
+        <v>905</v>
+      </c>
+      <c r="K1526" s="26">
+        <v>6</v>
+      </c>
+      <c r="L1526" s="11"/>
+      <c r="M1526" s="10"/>
+      <c r="N1526" s="10" t="str">
+        <f t="shared" si="234"/>
+        <v>ge11_af_auto_out_of_range_6</v>
+      </c>
+      <c r="O1526" s="3" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="1527" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1527" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1527" s="9">
+        <v>54</v>
+      </c>
+      <c r="C1527" s="9">
+        <v>0</v>
+      </c>
+      <c r="D1527" s="9">
+        <v>73</v>
+      </c>
+      <c r="E1527" s="10" t="str">
+        <f t="shared" si="233"/>
+        <v>000B6398</v>
+      </c>
+      <c r="F1527" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1527" s="8" t="s">
+        <v>912</v>
+      </c>
+      <c r="H1527" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1527" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1527" s="16" t="s">
+        <v>911</v>
+      </c>
+      <c r="K1527" s="26">
+        <v>0</v>
+      </c>
+      <c r="L1527" s="11"/>
+      <c r="M1527" s="10"/>
+      <c r="N1527" s="10" t="str">
+        <f t="shared" si="234"/>
+        <v>ge11_bc0_period_err_0</v>
+      </c>
+      <c r="O1527" s="3" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="1528" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1528" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1528" s="9">
+        <v>54</v>
+      </c>
+      <c r="C1528" s="9">
+        <v>0</v>
+      </c>
+      <c r="D1528" s="9">
+        <v>73</v>
+      </c>
+      <c r="E1528" s="10" t="str">
+        <f t="shared" si="233"/>
+        <v>000B6398</v>
+      </c>
+      <c r="F1528" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1528" s="8" t="s">
+        <v>913</v>
+      </c>
+      <c r="H1528" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1528" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1528" s="16" t="s">
+        <v>911</v>
+      </c>
+      <c r="K1528" s="26">
+        <v>1</v>
+      </c>
+      <c r="L1528" s="11"/>
+      <c r="M1528" s="10"/>
+      <c r="N1528" s="10" t="str">
+        <f t="shared" si="234"/>
+        <v>ge11_bc0_period_err_1</v>
+      </c>
+      <c r="O1528" s="3" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="1529" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1529" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1529" s="9">
+        <v>54</v>
+      </c>
+      <c r="C1529" s="9">
+        <v>0</v>
+      </c>
+      <c r="D1529" s="9">
+        <v>73</v>
+      </c>
+      <c r="E1529" s="10" t="str">
+        <f t="shared" ref="E1529:E1533" si="235">DEC2HEX(HEX2DEC(A1529)+B1529*4096+HEX2DEC(D1529)*8,8)</f>
+        <v>000B6398</v>
+      </c>
+      <c r="F1529" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1529" s="8" t="s">
+        <v>914</v>
+      </c>
+      <c r="H1529" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1529" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1529" s="16" t="s">
+        <v>911</v>
+      </c>
+      <c r="K1529" s="26">
+        <v>2</v>
+      </c>
+      <c r="L1529" s="11"/>
+      <c r="M1529" s="10"/>
+      <c r="N1529" s="10" t="str">
+        <f t="shared" ref="N1529:N1533" si="236">CONCATENATE(O1529,"_",K1529)</f>
+        <v>ge11_bc0_period_err_2</v>
+      </c>
+      <c r="O1529" s="3" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="1530" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1530" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1530" s="9">
+        <v>54</v>
+      </c>
+      <c r="C1530" s="9">
+        <v>0</v>
+      </c>
+      <c r="D1530" s="9">
+        <v>73</v>
+      </c>
+      <c r="E1530" s="10" t="str">
+        <f t="shared" si="235"/>
+        <v>000B6398</v>
+      </c>
+      <c r="F1530" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1530" s="8" t="s">
+        <v>915</v>
+      </c>
+      <c r="H1530" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1530" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1530" s="16" t="s">
+        <v>911</v>
+      </c>
+      <c r="K1530" s="26">
+        <v>3</v>
+      </c>
+      <c r="L1530" s="11"/>
+      <c r="M1530" s="10"/>
+      <c r="N1530" s="10" t="str">
+        <f t="shared" si="236"/>
+        <v>ge11_bc0_period_err_3</v>
+      </c>
+      <c r="O1530" s="3" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="1531" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1531" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1531" s="9">
+        <v>54</v>
+      </c>
+      <c r="C1531" s="9">
+        <v>0</v>
+      </c>
+      <c r="D1531" s="9">
+        <v>73</v>
+      </c>
+      <c r="E1531" s="10" t="str">
+        <f t="shared" si="235"/>
+        <v>000B6398</v>
+      </c>
+      <c r="F1531" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1531" s="8" t="s">
+        <v>916</v>
+      </c>
+      <c r="H1531" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1531" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1531" s="16" t="s">
+        <v>911</v>
+      </c>
+      <c r="K1531" s="26">
+        <v>4</v>
+      </c>
+      <c r="L1531" s="11"/>
+      <c r="M1531" s="10"/>
+      <c r="N1531" s="10" t="str">
+        <f t="shared" si="236"/>
+        <v>ge11_bc0_period_err_4</v>
+      </c>
+      <c r="O1531" s="3" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="1532" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1532" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1532" s="9">
+        <v>54</v>
+      </c>
+      <c r="C1532" s="9">
+        <v>0</v>
+      </c>
+      <c r="D1532" s="9">
+        <v>73</v>
+      </c>
+      <c r="E1532" s="10" t="str">
+        <f t="shared" si="235"/>
+        <v>000B6398</v>
+      </c>
+      <c r="F1532" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1532" s="8" t="s">
+        <v>917</v>
+      </c>
+      <c r="H1532" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1532" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1532" s="16" t="s">
+        <v>911</v>
+      </c>
+      <c r="K1532" s="26">
+        <v>5</v>
+      </c>
+      <c r="L1532" s="11"/>
+      <c r="M1532" s="10"/>
+      <c r="N1532" s="10" t="str">
+        <f t="shared" si="236"/>
+        <v>ge11_bc0_period_err_5</v>
+      </c>
+      <c r="O1532" s="3" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="1533" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1533" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1533" s="9">
+        <v>54</v>
+      </c>
+      <c r="C1533" s="9">
+        <v>0</v>
+      </c>
+      <c r="D1533" s="9">
+        <v>73</v>
+      </c>
+      <c r="E1533" s="10" t="str">
+        <f t="shared" si="235"/>
+        <v>000B6398</v>
+      </c>
+      <c r="F1533" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1533" s="8" t="s">
+        <v>918</v>
+      </c>
+      <c r="H1533" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1533" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1533" s="16" t="s">
+        <v>911</v>
+      </c>
+      <c r="K1533" s="26">
+        <v>6</v>
+      </c>
+      <c r="L1533" s="11"/>
+      <c r="M1533" s="10"/>
+      <c r="N1533" s="10" t="str">
+        <f t="shared" si="236"/>
+        <v>ge11_bc0_period_err_6</v>
+      </c>
+      <c r="O1533" s="3" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="1534" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1534" s="8"/>
+      <c r="B1534" s="9"/>
+      <c r="C1534" s="9"/>
+      <c r="D1534" s="9"/>
+      <c r="E1534" s="10"/>
+      <c r="F1534" s="8"/>
+      <c r="G1534" s="8"/>
+      <c r="H1534" s="8"/>
+      <c r="I1534" s="18"/>
+      <c r="J1534" s="29"/>
+      <c r="K1534" s="30"/>
+      <c r="L1534" s="11"/>
+      <c r="M1534" s="10"/>
+      <c r="N1534" s="10"/>
+    </row>
+    <row r="1535" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1535" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1535" s="9">
+        <v>54</v>
+      </c>
+      <c r="C1535" s="9">
+        <v>0</v>
+      </c>
+      <c r="D1535" s="9">
+        <v>74</v>
+      </c>
+      <c r="E1535" s="10" t="str">
+        <f t="shared" ref="E1535:E1536" si="237">DEC2HEX(HEX2DEC(A1535)+B1535*4096+HEX2DEC(D1535)*8,8)</f>
+        <v>000B63A0</v>
+      </c>
+      <c r="F1535" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1535" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1535" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1535" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1535" s="16" t="s">
+        <v>921</v>
+      </c>
+      <c r="K1535" s="26"/>
+      <c r="L1535" s="11"/>
+      <c r="M1535" s="10"/>
+      <c r="N1535" s="3" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1536" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1536" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1536" s="9">
+        <v>54</v>
+      </c>
+      <c r="C1536" s="9">
+        <v>0</v>
+      </c>
+      <c r="D1536" s="9">
+        <v>74</v>
+      </c>
+      <c r="E1536" s="10" t="str">
+        <f t="shared" si="237"/>
+        <v>000B63A0</v>
+      </c>
+      <c r="F1536" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1536" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="H1536" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1536" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1536" s="16" t="s">
+        <v>922</v>
+      </c>
+      <c r="K1536" s="26"/>
+      <c r="L1536" s="11"/>
+      <c r="M1536" s="10"/>
+      <c r="N1536" s="3" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="1537" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1537" s="8"/>
+      <c r="B1537" s="9"/>
+      <c r="C1537" s="9"/>
+      <c r="D1537" s="9"/>
+      <c r="E1537" s="10"/>
+      <c r="F1537" s="8"/>
+      <c r="G1537" s="8"/>
+      <c r="H1537" s="8"/>
+      <c r="I1537" s="18"/>
+      <c r="J1537" s="29"/>
+      <c r="K1537" s="30"/>
+      <c r="L1537" s="11"/>
+      <c r="M1537" s="10"/>
+      <c r="N1537" s="10"/>
+    </row>
+    <row r="1538" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1538" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1538" s="9">
+        <v>55</v>
+      </c>
+      <c r="C1538" s="9">
+        <v>0</v>
+      </c>
+      <c r="D1538" s="9">
+        <v>0</v>
+      </c>
+      <c r="E1538" s="10" t="str">
+        <f t="shared" ref="E1538" si="238">DEC2HEX(HEX2DEC(A1538)+B1538*4096+HEX2DEC(D1538)*8,8)</f>
+        <v>000B7000</v>
+      </c>
+      <c r="F1538" s="8" t="s">
+        <v>885</v>
+      </c>
+      <c r="G1538" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1538" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1538" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1538" s="16" t="s">
+        <v>883</v>
+      </c>
+      <c r="K1538" s="26"/>
+      <c r="L1538" s="11"/>
+      <c r="M1538" s="10"/>
+      <c r="N1538" s="10" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="1539" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1539" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1539" s="9">
+        <v>56</v>
+      </c>
+      <c r="C1539" s="9">
+        <v>0</v>
+      </c>
+      <c r="D1539" s="9">
+        <v>0</v>
+      </c>
+      <c r="E1539" s="10" t="str">
+        <f t="shared" ref="E1539" si="239">DEC2HEX(HEX2DEC(A1539)+B1539*4096+HEX2DEC(D1539)*8,8)</f>
+        <v>000B8000</v>
+      </c>
+      <c r="F1539" s="8" t="s">
+        <v>885</v>
+      </c>
+      <c r="G1539" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1539" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1539" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1539" s="16" t="s">
+        <v>886</v>
+      </c>
+      <c r="K1539" s="26"/>
+      <c r="L1539" s="11"/>
+      <c r="M1539" s="10"/>
+      <c r="N1539" s="10" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="1540" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1540" s="8"/>
+      <c r="B1540" s="9"/>
+      <c r="C1540" s="9"/>
+      <c r="D1540" s="9"/>
+      <c r="E1540" s="10"/>
+      <c r="F1540" s="8"/>
+      <c r="G1540" s="10"/>
+      <c r="H1540" s="8"/>
+      <c r="I1540" s="8"/>
+      <c r="J1540" s="8"/>
+      <c r="K1540" s="10"/>
+      <c r="L1540" s="11"/>
+      <c r="M1540" s="10"/>
+      <c r="N1540" s="10"/>
+    </row>
+    <row r="1541" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1541" s="8" t="s">
+        <v>859</v>
+      </c>
+      <c r="B1541" s="9"/>
+      <c r="C1541" s="9"/>
+      <c r="D1541" s="8"/>
+      <c r="E1541" s="10" t="s">
+        <v>860</v>
+      </c>
+      <c r="F1541" s="8" t="s">
+        <v>861</v>
+      </c>
+      <c r="G1541" s="8" t="s">
+        <v>862</v>
+      </c>
+      <c r="H1541" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1541" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1541" s="8" t="s">
+        <v>863</v>
+      </c>
+      <c r="K1541" s="10"/>
+      <c r="L1541" s="8"/>
+      <c r="M1541" s="10"/>
+      <c r="N1541" s="10" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="1542" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1542" s="8" t="s">
+        <v>859</v>
+      </c>
+      <c r="B1542" s="9"/>
+      <c r="C1542" s="9"/>
+      <c r="D1542" s="8"/>
+      <c r="E1542" s="8" t="s">
+        <v>865</v>
+      </c>
+      <c r="F1542" s="8" t="s">
+        <v>861</v>
+      </c>
+      <c r="G1542" s="8" t="s">
+        <v>862</v>
+      </c>
+      <c r="H1542" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1542" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1542" s="8" t="s">
+        <v>866</v>
+      </c>
+      <c r="K1542" s="10"/>
+      <c r="L1542" s="8"/>
+      <c r="M1542" s="10"/>
+      <c r="N1542" s="10" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="1543" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1543" s="8"/>
+      <c r="B1543" s="9"/>
+      <c r="C1543" s="9"/>
+      <c r="D1543" s="8"/>
+      <c r="E1543" s="10"/>
+      <c r="F1543" s="8"/>
+      <c r="G1543" s="8"/>
+      <c r="H1543" s="8"/>
+      <c r="I1543" s="8"/>
+      <c r="J1543" s="8"/>
+      <c r="K1543" s="10"/>
+      <c r="L1543" s="8"/>
+      <c r="M1543" s="10"/>
+      <c r="N1543" s="10"/>
+    </row>
+    <row r="1544" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1544" s="8" t="s">
+        <v>868</v>
+      </c>
+      <c r="B1544" s="9"/>
+      <c r="C1544" s="9"/>
+      <c r="D1544" s="8"/>
+      <c r="E1544" s="8" t="s">
+        <v>869</v>
+      </c>
+      <c r="F1544" s="8" t="s">
+        <v>870</v>
+      </c>
+      <c r="G1544" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1544" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1544" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1544" s="8" t="s">
+        <v>871</v>
+      </c>
+      <c r="K1544" s="10"/>
+      <c r="L1544" s="8"/>
+      <c r="M1544" s="10"/>
+      <c r="N1544" s="10" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="1545" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1545" s="8"/>
+      <c r="B1545" s="9"/>
+      <c r="C1545" s="9"/>
+      <c r="D1545" s="8"/>
+      <c r="E1545" s="10"/>
+      <c r="F1545" s="8"/>
+      <c r="G1545" s="8"/>
+      <c r="H1545" s="8"/>
+      <c r="I1545" s="8"/>
+      <c r="J1545" s="8"/>
+      <c r="K1545" s="10"/>
+      <c r="L1545" s="8"/>
+      <c r="M1545" s="10"/>
+      <c r="N1545" s="10"/>
+    </row>
+    <row r="1546" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1546" s="23"/>
+      <c r="B1546" s="27"/>
+      <c r="C1546" s="27"/>
+      <c r="D1546" s="23"/>
+      <c r="E1546" s="23" t="s">
         <v>873</v>
       </c>
-      <c r="F1513" s="23" t="s">
+      <c r="F1546" s="23" t="s">
         <v>874</v>
       </c>
-      <c r="G1513" s="23" t="s">
+      <c r="G1546" s="23" t="s">
         <v>875</v>
       </c>
-      <c r="H1513" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1513" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1513" s="23" t="s">
+      <c r="H1546" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1546" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1546" s="23" t="s">
         <v>876</v>
       </c>
-      <c r="K1513" s="23"/>
-      <c r="L1513" s="23"/>
-      <c r="M1513" s="23"/>
-      <c r="N1513" s="23" t="s">
+      <c r="K1546" s="23"/>
+      <c r="L1546" s="23"/>
+      <c r="M1546" s="23"/>
+      <c r="N1546" s="23" t="s">
         <v>877</v>
       </c>
     </row>
-    <row r="1514" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1514" s="24"/>
-      <c r="B1514" s="20"/>
-      <c r="C1514" s="20"/>
-      <c r="D1514" s="24"/>
-      <c r="E1514" s="24" t="s">
+    <row r="1547" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1547" s="24"/>
+      <c r="B1547" s="20"/>
+      <c r="C1547" s="20"/>
+      <c r="D1547" s="24"/>
+      <c r="E1547" s="24" t="s">
         <v>878</v>
       </c>
-      <c r="F1514" s="24" t="s">
+      <c r="F1547" s="24" t="s">
         <v>879</v>
       </c>
-      <c r="G1514" s="24" t="s">
+      <c r="G1547" s="24" t="s">
         <v>880</v>
       </c>
-      <c r="H1514" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1514" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1514" s="24" t="s">
+      <c r="H1547" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1547" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1547" s="24" t="s">
         <v>881</v>
       </c>
-      <c r="K1514" s="16"/>
-      <c r="L1514" s="24"/>
-      <c r="M1514" s="16"/>
-      <c r="N1514" s="16" t="s">
+      <c r="K1547" s="16"/>
+      <c r="L1547" s="24"/>
+      <c r="M1547" s="16"/>
+      <c r="N1547" s="16" t="s">
         <v>882</v>
       </c>
     </row>

</xml_diff>